<commit_message>
renaming funcs, changing column logic, add asserts in tests
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Container_creation_empty_row_v4_2_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Container_creation_empty_row_v4_2_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7CEE5D-9E1C-F54A-9275-43AF9465B70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEA0411-D1E8-9A42-897E-94726167F2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Container Creation Template</t>
   </si>
@@ -168,12 +168,15 @@
   <si>
     <t>vv</t>
   </si>
+  <si>
+    <t>zz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -226,6 +229,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -389,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -425,6 +434,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -822,37 +832,37 @@
     <col min="7" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -872,7 +882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -886,7 +896,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
@@ -901,8 +911,11 @@
       <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="J9" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -920,7 +933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -938,7 +951,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -946,7 +959,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -954,7 +967,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -962,7 +975,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -970,7 +983,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>

</xml_diff>

<commit_message>
adding to test template
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Container_creation_empty_row_v4_2_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Container_creation_empty_row_v4_2_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEA0411-D1E8-9A42-897E-94726167F2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A0A427-BAB7-2143-B4EA-87A8A7B2F1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Container Creation Template</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>zz</t>
+  </si>
+  <si>
+    <t>lo</t>
   </si>
 </sst>
 </file>
@@ -817,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -832,37 +835,37 @@
     <col min="7" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -882,7 +885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -896,7 +899,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
@@ -915,7 +918,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -933,7 +936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -950,8 +953,11 @@
         <v>23</v>
       </c>
       <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K11" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -959,15 +965,18 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="I13" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -975,7 +984,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -983,7 +992,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>

</xml_diff>